<commit_message>
add templates-ts and fix structure
</commit_message>
<xml_diff>
--- a/VivelTestExample.xlsx
+++ b/VivelTestExample.xlsx
@@ -20,15 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
   <si>
     <t xml:space="preserve">Character(s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Line(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Option(s)</t>
+    <t xml:space="preserve">Line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goTo</t>
   </si>
   <si>
     <t xml:space="preserve">Tom(Happy), Charlie(sad), </t>
@@ -37,6 +46,12 @@
     <t xml:space="preserve">Hello, there.</t>
   </si>
   <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom,</t>
+  </si>
+  <si>
     <t xml:space="preserve">This is an intro to Vivel</t>
   </si>
   <si>
@@ -65,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">ok then..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iklan</t>
   </si>
   <si>
     <t xml:space="preserve">Tom(Happy), Charlie(Happy), </t>
@@ -104,15 +122,15 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
+      <sz val="10"/>
+      <name val="Noto Mono"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Noto Mono"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -159,12 +177,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -189,21 +211,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57.94"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -212,74 +234,135 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>10</v>
-      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>13</v>
-      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>14</v>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>16</v>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make character overlap each other, add character example on cosmos
</commit_message>
<xml_diff>
--- a/VivelTestExample.xlsx
+++ b/VivelTestExample.xlsx
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Really ???</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes, of course.. we can have fun later on</t>
+    <t xml:space="preserve">Wisnu Jelek</t>
   </si>
   <si>
     <t xml:space="preserve">ok then..</t>
@@ -211,7 +211,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D11"/>
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>